<commit_message>
new research and protection analysis
</commit_message>
<xml_diff>
--- a/ReflectionsAndData/csv/charts.xlsx
+++ b/ReflectionsAndData/csv/charts.xlsx
@@ -4,13 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30080" windowHeight="19340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="260" yWindow="0" windowWidth="32320" windowHeight="19340" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="19" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>level 1</t>
   </si>
@@ -84,6 +89,45 @@
   <si>
     <t>highest level 6</t>
   </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Minutes Played</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>ac</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>average research time</t>
+  </si>
+  <si>
+    <t>average protection %</t>
+  </si>
 </sst>
 </file>
 
@@ -131,8 +175,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -142,9 +188,11 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -528,11 +576,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2069594568"/>
-        <c:axId val="2069601544"/>
+        <c:axId val="2120331656"/>
+        <c:axId val="2120338856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2069594568"/>
+        <c:axId val="2120331656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +612,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069601544"/>
+        <c:crossAx val="2120338856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -572,7 +620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2069601544"/>
+        <c:axId val="2120338856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -602,7 +650,514 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069594568"/>
+        <c:crossAx val="2120331656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$E$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>level 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$A$10:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>nil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>c</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ab</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>bc</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>abc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$E$10:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>403.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>347.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>648.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>676.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>238.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>880.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1835.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2131881640"/>
+        <c:axId val="-2132110040"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2131881640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2132110040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2132110040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2131881640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$F$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>level 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$A$10:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>nil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>c</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ab</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>bc</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>abc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$F$10:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>225.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>114.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>289.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>322.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>371.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>739.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2133868936"/>
+        <c:axId val="-2134159656"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2133868936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2134159656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2134159656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2133868936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$G$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>level 6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$A$10:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>nil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>c</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ab</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>bc</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>abc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$G$10:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>179.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2134274296"/>
+        <c:axId val="-2133376184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2134274296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2133376184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2133376184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2134274296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1000,11 +1555,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2069673016"/>
-        <c:axId val="2069678744"/>
+        <c:axId val="2119726888"/>
+        <c:axId val="2119732616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2069673016"/>
+        <c:axId val="2119726888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,7 +1587,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069678744"/>
+        <c:crossAx val="2119732616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1040,7 +1595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2069678744"/>
+        <c:axId val="2119732616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1070,7 +1625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069673016"/>
+        <c:crossAx val="2119726888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1433,11 +1988,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2076344696"/>
-        <c:axId val="2076346968"/>
+        <c:axId val="2119784296"/>
+        <c:axId val="2119789960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2076344696"/>
+        <c:axId val="2119784296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,7 +2021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076346968"/>
+        <c:crossAx val="2119789960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1474,7 +2029,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2076346968"/>
+        <c:axId val="2119789960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,7 +2064,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076344696"/>
+        <c:crossAx val="2119784296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1872,11 +2427,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2130916824"/>
-        <c:axId val="2130923608"/>
+        <c:axId val="2119833704"/>
+        <c:axId val="2119839368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2130916824"/>
+        <c:axId val="2119833704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,7 +2460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130923608"/>
+        <c:crossAx val="2119839368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1913,7 +2468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130923608"/>
+        <c:axId val="2119839368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,7 +2503,912 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130916824"/>
+        <c:crossAx val="2119833704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>average research time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$19:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$19:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2129738728"/>
+        <c:axId val="-2126890424"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2129738728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Highest level reached</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2126890424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2126890424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average research time per level (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2129738728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>average protection %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$A$27:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$27:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2132119224"/>
+        <c:axId val="-2125274888"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2132119224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Highest level reached</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2125274888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2125274888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> protection % at end of level</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2132119224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>level 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$A$10:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>nil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>c</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ab</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>bc</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>abc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$B$10:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3335.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1864.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2280.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9234.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2367.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1815.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6009.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11248.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2129367608"/>
+        <c:axId val="-2132012408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2129367608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2132012408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2132012408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2129367608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>level 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$A$10:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>nil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>c</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ab</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>bc</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>abc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$C$10:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1427.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1163.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>962.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4200.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2013.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1317.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4133.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8776.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2129212648"/>
+        <c:axId val="-2132157416"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2129212648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2132157416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2132157416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2129212648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet7!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>level 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet7!$A$10:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>nil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>c</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ab</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>bc</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>abc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet7!$D$10:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>658.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>652.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>443.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1837.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1215.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>573.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2132.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4564.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2134084792"/>
+        <c:axId val="-2133266264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2134084792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2133266264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2133266264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2134084792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2039,16 +3499,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2069,16 +3529,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2097,7 +3557,365 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Information Technology" refreshedDate="41981.559038078703" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="5">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B1:G6" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="level 1" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="52" maxValue="390" count="5">
+        <n v="390"/>
+        <n v="317"/>
+        <n v="107"/>
+        <n v="81"/>
+        <n v="52"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="level 2" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="232" maxValue="456"/>
+    </cacheField>
+    <cacheField name="level 3" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="166" maxValue="405"/>
+    </cacheField>
+    <cacheField name="level 4" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="194" maxValue="349"/>
+    </cacheField>
+    <cacheField name="level 5" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="145" maxValue="336"/>
+    </cacheField>
+    <cacheField name="level 6" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="86" maxValue="125"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="5">
+  <r>
+    <x v="0"/>
+    <n v="232"/>
+    <n v="166"/>
+    <n v="194"/>
+    <n v="174"/>
+    <n v="98"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="456"/>
+    <n v="363"/>
+    <n v="315"/>
+    <n v="336"/>
+    <n v="125"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="241"/>
+    <n v="300"/>
+    <n v="204"/>
+    <n v="191"/>
+    <n v="86"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="261"/>
+    <n v="232"/>
+    <n v="197"/>
+    <n v="145"/>
+    <n v="92"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="296"/>
+    <n v="405"/>
+    <n v="349"/>
+    <n v="201"/>
+    <n v="88"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:F16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2422,10 +4240,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N15:N16"/>
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2566,6 +4406,9 @@
       </c>
     </row>
     <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -2711,17 +4554,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -2820,6 +4666,9 @@
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -2915,6 +4764,538 @@
       </c>
       <c r="F15">
         <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>3335</v>
+      </c>
+      <c r="C2">
+        <v>1864</v>
+      </c>
+      <c r="D2">
+        <v>2280</v>
+      </c>
+      <c r="E2">
+        <v>9234</v>
+      </c>
+      <c r="F2">
+        <v>2367</v>
+      </c>
+      <c r="G2">
+        <v>1815</v>
+      </c>
+      <c r="H2">
+        <v>6009</v>
+      </c>
+      <c r="I2">
+        <v>11248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1427</v>
+      </c>
+      <c r="C3">
+        <v>1163</v>
+      </c>
+      <c r="D3">
+        <v>962</v>
+      </c>
+      <c r="E3">
+        <v>4200</v>
+      </c>
+      <c r="F3">
+        <v>2013</v>
+      </c>
+      <c r="G3">
+        <v>1317</v>
+      </c>
+      <c r="H3">
+        <v>4133</v>
+      </c>
+      <c r="I3">
+        <v>8776</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>658</v>
+      </c>
+      <c r="C4">
+        <v>652</v>
+      </c>
+      <c r="D4">
+        <v>443</v>
+      </c>
+      <c r="E4">
+        <v>1837</v>
+      </c>
+      <c r="F4">
+        <v>1215</v>
+      </c>
+      <c r="G4">
+        <v>573</v>
+      </c>
+      <c r="H4">
+        <v>2132</v>
+      </c>
+      <c r="I4">
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>403</v>
+      </c>
+      <c r="C5">
+        <v>347</v>
+      </c>
+      <c r="D5">
+        <v>220</v>
+      </c>
+      <c r="E5">
+        <v>648</v>
+      </c>
+      <c r="F5">
+        <v>676</v>
+      </c>
+      <c r="G5">
+        <v>238</v>
+      </c>
+      <c r="H5">
+        <v>880</v>
+      </c>
+      <c r="I5">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>225</v>
+      </c>
+      <c r="C6">
+        <v>190</v>
+      </c>
+      <c r="D6">
+        <v>114</v>
+      </c>
+      <c r="E6">
+        <v>289</v>
+      </c>
+      <c r="F6">
+        <v>322</v>
+      </c>
+      <c r="G6">
+        <v>110</v>
+      </c>
+      <c r="H6">
+        <v>371</v>
+      </c>
+      <c r="I6">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>96</v>
+      </c>
+      <c r="F7">
+        <v>89</v>
+      </c>
+      <c r="G7">
+        <v>41</v>
+      </c>
+      <c r="H7">
+        <v>92</v>
+      </c>
+      <c r="I7">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>3335</v>
+      </c>
+      <c r="C10">
+        <v>1427</v>
+      </c>
+      <c r="D10">
+        <v>658</v>
+      </c>
+      <c r="E10">
+        <v>403</v>
+      </c>
+      <c r="F10">
+        <v>225</v>
+      </c>
+      <c r="G10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>1864</v>
+      </c>
+      <c r="C11">
+        <v>1163</v>
+      </c>
+      <c r="D11">
+        <v>652</v>
+      </c>
+      <c r="E11">
+        <v>347</v>
+      </c>
+      <c r="F11">
+        <v>190</v>
+      </c>
+      <c r="G11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>2280</v>
+      </c>
+      <c r="C12">
+        <v>962</v>
+      </c>
+      <c r="D12">
+        <v>443</v>
+      </c>
+      <c r="E12">
+        <v>220</v>
+      </c>
+      <c r="F12">
+        <v>114</v>
+      </c>
+      <c r="G12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>9234</v>
+      </c>
+      <c r="C13">
+        <v>4200</v>
+      </c>
+      <c r="D13">
+        <v>1837</v>
+      </c>
+      <c r="E13">
+        <v>648</v>
+      </c>
+      <c r="F13">
+        <v>289</v>
+      </c>
+      <c r="G13">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>2367</v>
+      </c>
+      <c r="C14">
+        <v>2013</v>
+      </c>
+      <c r="D14">
+        <v>1215</v>
+      </c>
+      <c r="E14">
+        <v>676</v>
+      </c>
+      <c r="F14">
+        <v>322</v>
+      </c>
+      <c r="G14">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>1815</v>
+      </c>
+      <c r="C15">
+        <v>1317</v>
+      </c>
+      <c r="D15">
+        <v>573</v>
+      </c>
+      <c r="E15">
+        <v>238</v>
+      </c>
+      <c r="F15">
+        <v>110</v>
+      </c>
+      <c r="G15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>6009</v>
+      </c>
+      <c r="C16">
+        <v>4133</v>
+      </c>
+      <c r="D16">
+        <v>2132</v>
+      </c>
+      <c r="E16">
+        <v>880</v>
+      </c>
+      <c r="F16">
+        <v>371</v>
+      </c>
+      <c r="G16">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>11248</v>
+      </c>
+      <c r="C17">
+        <v>8776</v>
+      </c>
+      <c r="D17">
+        <v>4564</v>
+      </c>
+      <c r="E17">
+        <v>1835</v>
+      </c>
+      <c r="F17">
+        <v>739</v>
+      </c>
+      <c r="G17">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>